<commit_message>
Update nutrients file with new data, minor work on functions and notebook
</commit_message>
<xml_diff>
--- a/MUDBENCS_2023_Nuts_Results v2.xlsx
+++ b/MUDBENCS_2023_Nuts_Results v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beros\Box\UDrive_brosenheim\My_Documents\PyCode\MUDBENCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brosenheim\Box\UDrive_brosenheim\My_Documents\PyCode\MUDBENCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{31B40A01-9918-4EC6-BCDC-6D359AA4E19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E7E2D20-7255-4197-A6AE-085A44D91E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{2FAAE085-B789-4EE2-BB7A-0322FD7400E9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{2FAAE085-B789-4EE2-BB7A-0322FD7400E9}"/>
   </bookViews>
   <sheets>
     <sheet name="MUDBENCS Results" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="81">
   <si>
     <t>SAMPLES</t>
   </si>
@@ -84,9 +84,6 @@
     <t>MUDBENCS 1</t>
   </si>
   <si>
-    <t>&lt;LOD</t>
-  </si>
-  <si>
     <t>STD5</t>
   </si>
   <si>
@@ -249,9 +246,6 @@
     <t>STN17 SW INT</t>
   </si>
   <si>
-    <t>STN 15</t>
-  </si>
-  <si>
     <t>STN21</t>
   </si>
   <si>
@@ -301,6 +295,9 @@
   </si>
   <si>
     <t>1:4 dilution</t>
+  </si>
+  <si>
+    <t>STN15</t>
   </si>
 </sst>
 </file>
@@ -422,9 +419,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -462,7 +459,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -568,7 +565,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -710,7 +707,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -728,18 +725,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E665195-887C-4057-B971-DCEBB3AB647A}">
   <dimension ref="A1:Z81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.46484375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -755,7 +752,7 @@
       <c r="K1" s="10"/>
       <c r="L1" s="10"/>
       <c r="O1" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P1" s="10"/>
       <c r="Q1" s="10"/>
@@ -769,7 +766,7 @@
       <c r="Y1" s="10"/>
       <c r="Z1" s="10"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -777,7 +774,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>6</v>
@@ -789,7 +786,7 @@
         <v>4</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>6</v>
@@ -802,7 +799,7 @@
         <v>4</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>6</v>
@@ -814,13 +811,13 @@
         <v>4</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Z2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
@@ -871,32 +868,32 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="4">
-        <v>5.5E-2</v>
-      </c>
-      <c r="C5" s="4" t="s">
+        <v>0.01</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.26</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.52100000000000002</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="I5" s="4">
         <v>0.49099999999999999</v>
@@ -911,7 +908,7 @@
         <v>0.21</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="P5" s="4">
         <v>1.46</v>
@@ -926,7 +923,7 @@
         <v>0.12</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W5" s="4">
         <v>4.9000000000000002E-2</v>
@@ -941,24 +938,24 @@
         <v>0.55800000000000005</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="4">
-        <v>0.57399999999999995</v>
+        <v>0.435</v>
       </c>
       <c r="C6" s="4">
-        <v>16.678999999999998</v>
+        <v>13.5</v>
       </c>
       <c r="D6" s="8">
-        <v>131.93199999999999</v>
-      </c>
-      <c r="E6" s="4" t="s">
+        <v>125.765</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="I6" s="4">
         <v>0.48299999999999998</v>
@@ -985,7 +982,7 @@
         <v>0.124</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W6" s="4">
         <v>4.3999999999999997E-2</v>
@@ -1000,24 +997,24 @@
         <v>0.51200000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="4">
-        <v>0.39400000000000002</v>
+        <v>0.36499999999999999</v>
       </c>
       <c r="C7" s="4">
-        <v>19.544</v>
+        <v>16.314999999999998</v>
       </c>
       <c r="D7" s="8">
-        <v>119.184</v>
+        <v>111.37</v>
       </c>
       <c r="E7" s="4">
-        <v>0.17799999999999999</v>
+        <v>0.1</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I7" s="4">
         <v>0.51700000000000002</v>
@@ -1044,7 +1041,7 @@
         <v>0.112</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W7" s="4">
         <v>5.2999999999999999E-2</v>
@@ -1059,24 +1056,24 @@
         <v>0.55700000000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="4">
-        <v>0.54800000000000004</v>
+        <v>0.49</v>
       </c>
       <c r="C8" s="4">
-        <v>18.905999999999999</v>
+        <v>13.79</v>
       </c>
       <c r="D8" s="8">
-        <v>132.41200000000001</v>
-      </c>
-      <c r="E8" s="4" t="s">
+        <v>119.005</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="I8" s="4">
         <v>0.50900000000000001</v>
@@ -1091,7 +1088,7 @@
         <v>0.20799999999999999</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W8" s="4">
         <v>4.5999999999999999E-2</v>
@@ -1106,24 +1103,24 @@
         <v>0.48899999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="4">
-        <v>0.55700000000000005</v>
+        <v>0.4</v>
       </c>
       <c r="C9" s="4">
-        <v>9.7629999999999999</v>
+        <v>7.9950000000000001</v>
       </c>
       <c r="D9" s="4">
-        <v>42.99</v>
-      </c>
-      <c r="E9" s="4" t="s">
+        <v>42.370000000000005</v>
+      </c>
+      <c r="E9" s="4">
+        <v>5.5E-2</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="I9" s="4">
         <v>0.50900000000000001</v>
@@ -1138,7 +1135,7 @@
         <v>0.19600000000000001</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P9" s="4">
         <f>AVERAGE(P5:P7)</f>
@@ -1157,7 +1154,7 @@
         <v>0.11866666666666666</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W9" s="4">
         <v>5.1999999999999998E-2</v>
@@ -1172,24 +1169,24 @@
         <v>0.48299999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="4">
-        <v>0.56000000000000005</v>
+        <v>0.54</v>
       </c>
       <c r="C10" s="4">
-        <v>2.7029999999999998</v>
+        <v>2.1550000000000002</v>
       </c>
       <c r="D10" s="4">
-        <v>39.302</v>
+        <v>38.784999999999997</v>
       </c>
       <c r="E10" s="4">
-        <v>0.12</v>
+        <v>7.5000000000000011E-2</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I10" s="4">
         <v>0.5</v>
@@ -1204,7 +1201,7 @@
         <v>0.20599999999999999</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P10" s="4">
         <f>_xlfn.STDEV.S(P5:P7)</f>
@@ -1227,24 +1224,24 @@
       <c r="Y10" s="4"/>
       <c r="Z10" s="4"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="4">
-        <v>0.255</v>
-      </c>
-      <c r="C11" s="4" t="s">
+        <v>0.02</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>12.315000000000001</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="D11" s="4">
-        <v>12.016999999999999</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="I11" s="4">
         <v>0.49199999999999999</v>
@@ -1259,7 +1256,7 @@
         <v>0.20699999999999999</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P11" s="4">
         <f>P10/P9*100</f>
@@ -1278,7 +1275,7 @@
         <v>5.1489614550065603</v>
       </c>
       <c r="V11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="W11" s="4">
         <f>AVERAGE(W5:W9)</f>
@@ -1297,24 +1294,24 @@
         <v>0.51980000000000004</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="4">
-        <v>0.247</v>
-      </c>
-      <c r="C12" s="4" t="s">
+        <v>0.02</v>
+      </c>
+      <c r="C12" s="4">
+        <v>8.4999999999999992E-2</v>
+      </c>
+      <c r="D12" s="4">
+        <v>25.405000000000001</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="D12" s="4">
-        <v>25.189</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="I12" s="4">
         <v>0.49199999999999999</v>
@@ -1329,7 +1326,7 @@
         <v>0.21</v>
       </c>
       <c r="V12" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="W12" s="4">
         <f>_xlfn.STDEV.S(W5:W9)</f>
@@ -1348,24 +1345,24 @@
         <v>3.6079079810882125E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="4">
-        <v>0.34</v>
+        <v>0.20500000000000002</v>
       </c>
       <c r="C13" s="4">
-        <v>0.90600000000000003</v>
+        <v>0</v>
       </c>
       <c r="D13" s="4">
-        <v>21.015000000000001</v>
+        <v>22.074999999999999</v>
       </c>
       <c r="E13" s="4">
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="V13" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="W13" s="4">
         <f>W12/W11*100</f>
@@ -1384,24 +1381,24 @@
         <v>6.9409541767760912</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="4">
-        <v>0.25900000000000001</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>9</v>
+        <v>0.18</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0</v>
       </c>
       <c r="D14" s="4">
-        <v>5.6429999999999998</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>9</v>
+        <v>5.3149999999999995</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I14" s="4">
         <f>AVERAGE(I4:I12)</f>
@@ -1420,31 +1417,31 @@
         <v>0.207875</v>
       </c>
       <c r="O14" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="P14" s="10"/>
       <c r="Q14" s="10"/>
       <c r="R14" s="10"/>
       <c r="S14" s="10"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="4">
-        <v>0.308</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>9</v>
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0</v>
       </c>
       <c r="D15" s="4">
-        <v>5.444</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>9</v>
+        <v>5.4</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I15" s="4">
         <f>_xlfn.STDEV.S(I4:I12)</f>
@@ -1463,24 +1460,24 @@
         <v>6.9165949508617095E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" s="4">
-        <v>0.154</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>9</v>
+        <v>0.1</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0</v>
       </c>
       <c r="D16" s="4">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>9</v>
+        <v>4.1550000000000002</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I16" s="4">
         <f>I15/I14*100</f>
@@ -1511,21 +1508,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" s="4">
-        <v>0.224</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="C17" s="4">
-        <v>0.58699999999999997</v>
+        <v>0.41</v>
       </c>
       <c r="D17" s="4">
-        <v>3.91</v>
+        <v>3.7249999999999996</v>
       </c>
       <c r="E17" s="4">
-        <v>0.23300000000000001</v>
+        <v>0.18</v>
       </c>
       <c r="P17" s="1" t="s">
         <v>7</v>
@@ -1540,7 +1537,7 @@
         <v>7</v>
       </c>
       <c r="V17" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W17" s="4">
         <v>0.71</v>
@@ -1555,24 +1552,24 @@
         <v>0.41899999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" s="4">
-        <v>0.374</v>
+        <v>0.315</v>
       </c>
       <c r="C18" s="4">
-        <v>0.69799999999999995</v>
+        <v>0.5</v>
       </c>
       <c r="D18" s="4">
-        <v>10.243</v>
+        <v>10.045</v>
       </c>
       <c r="E18" s="4">
-        <v>0.23899999999999999</v>
+        <v>0.17</v>
       </c>
       <c r="V18" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W18" s="4">
         <v>0.748</v>
@@ -1587,24 +1584,24 @@
         <v>0.45500000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" s="4">
-        <v>0.253</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>9</v>
+        <v>0.155</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0</v>
       </c>
       <c r="D19" s="4">
-        <v>14.648</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>9</v>
+        <v>15.395</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0</v>
       </c>
       <c r="O19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P19" s="5">
         <v>8.1055536516637765E-3</v>
@@ -1619,7 +1616,7 @@
         <v>2.8110496260293924E-2</v>
       </c>
       <c r="V19" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W19" s="4">
         <v>0.69</v>
@@ -1634,24 +1631,24 @@
         <v>0.39400000000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" s="4">
-        <v>0.255</v>
+        <v>5.5E-2</v>
       </c>
       <c r="C20" s="4">
-        <v>0.86099999999999999</v>
+        <v>0</v>
       </c>
       <c r="D20" s="4">
-        <v>5.0960000000000001</v>
+        <v>6.1050000000000004</v>
       </c>
       <c r="E20" s="4">
-        <v>0.32400000000000001</v>
+        <v>0</v>
       </c>
       <c r="V20" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W20" s="4">
         <v>0.77300000000000002</v>
@@ -1666,24 +1663,24 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="4">
-        <v>0.219</v>
+        <v>5.5E-2</v>
       </c>
       <c r="C21" s="4">
-        <v>1.6120000000000001</v>
+        <v>1.145</v>
       </c>
       <c r="D21" s="4">
-        <v>4.2279999999999998</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="E21" s="4">
-        <v>0.48599999999999999</v>
+        <v>0.46499999999999997</v>
       </c>
       <c r="V21" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W21" s="4">
         <v>0.83299999999999996</v>
@@ -1698,41 +1695,41 @@
         <v>0.378</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="4">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0</v>
+      </c>
+      <c r="D22" s="4">
+        <v>12.170000000000002</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="4">
-        <v>0.30599999999999999</v>
-      </c>
-      <c r="C22" s="4">
-        <v>0.49199999999999999</v>
-      </c>
-      <c r="D22" s="4">
-        <v>9.89</v>
-      </c>
-      <c r="E22" s="4">
-        <v>0.122</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A23" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="B23" s="4">
-        <v>0.13900000000000001</v>
+        <v>0.03</v>
       </c>
       <c r="C23" s="4">
-        <v>10.840999999999999</v>
+        <v>8.2899999999999991</v>
       </c>
       <c r="D23" s="4">
-        <v>101.65600000000001</v>
+        <v>164.97</v>
       </c>
       <c r="E23" s="4">
-        <v>0.47799999999999998</v>
+        <v>0</v>
       </c>
       <c r="V23" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="W23" s="4">
         <f>AVERAGE(W17:W21)</f>
@@ -1751,24 +1748,24 @@
         <v>0.4042</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B24" s="4">
-        <v>0.11700000000000001</v>
+        <v>0.01</v>
       </c>
       <c r="C24" s="4">
-        <v>0.16800000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="D24" s="4">
-        <v>0.77500000000000002</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>9</v>
+        <v>0.45</v>
+      </c>
+      <c r="E24" s="4">
+        <v>0</v>
       </c>
       <c r="V24" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="W24" s="4">
         <f>_xlfn.STDEV.S(W17:W21)</f>
@@ -1787,24 +1784,24 @@
         <v>3.3327166096144452E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" s="4">
-        <v>0.155</v>
+        <v>0.06</v>
       </c>
       <c r="C25" s="4">
-        <v>11.455</v>
+        <v>8.5500000000000007</v>
       </c>
       <c r="D25" s="8">
-        <v>96.662400000000005</v>
+        <v>166.38</v>
       </c>
       <c r="E25" s="4">
-        <v>0.58199999999999996</v>
+        <v>0</v>
       </c>
       <c r="V25" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="W25" s="4">
         <f>W24/W23*100</f>
@@ -1823,449 +1820,449 @@
         <v>8.245216748180221</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="C26" s="4">
+        <v>16.57</v>
+      </c>
+      <c r="D26" s="8">
+        <v>121.37</v>
+      </c>
+      <c r="E26" s="4">
+        <v>0.36499999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="4">
-        <v>0.45800000000000002</v>
-      </c>
-      <c r="C26" s="4">
-        <v>21.867000000000001</v>
-      </c>
-      <c r="D26" s="8">
-        <v>124.56</v>
-      </c>
-      <c r="E26" s="4">
-        <v>0.27500000000000002</v>
-      </c>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A27" s="2" t="s">
+      <c r="B27" s="4">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="C27" s="4">
+        <v>10.23</v>
+      </c>
+      <c r="D27" s="4">
+        <v>23.47</v>
+      </c>
+      <c r="E27" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="4">
-        <v>0.60099999999999998</v>
-      </c>
-      <c r="C27" s="4">
-        <v>10.106999999999999</v>
-      </c>
-      <c r="D27" s="4">
-        <v>19.379000000000001</v>
-      </c>
-      <c r="E27" s="4">
-        <v>4.5999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A28" s="2" t="s">
+      <c r="B28" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="C28" s="4">
+        <v>1.24</v>
+      </c>
+      <c r="D28" s="4">
+        <v>9.7100000000000009</v>
+      </c>
+      <c r="E28" s="4">
+        <v>0.61499999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="4">
-        <v>0.44</v>
-      </c>
-      <c r="C28" s="4">
-        <v>1.742</v>
-      </c>
-      <c r="D28" s="4">
-        <v>8.2590000000000003</v>
-      </c>
-      <c r="E28" s="4">
-        <v>0.40699999999999997</v>
-      </c>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A29" s="2" t="s">
+      <c r="B29" s="4">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="C29" s="4">
+        <v>9.44</v>
+      </c>
+      <c r="D29" s="4">
+        <v>45.585000000000001</v>
+      </c>
+      <c r="E29" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="4">
-        <v>0.50600000000000001</v>
-      </c>
-      <c r="C29" s="4">
-        <v>9.5869999999999997</v>
-      </c>
-      <c r="D29" s="4">
-        <v>43.149000000000001</v>
-      </c>
-      <c r="E29" s="4" t="s">
+      <c r="B30" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="C30" s="4">
+        <v>4.24</v>
+      </c>
+      <c r="D30" s="4">
+        <v>44.534999999999997</v>
+      </c>
+      <c r="E30" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="C31" s="4">
+        <v>0.42000000000000004</v>
+      </c>
+      <c r="D31" s="4">
+        <v>0.52499999999999991</v>
+      </c>
+      <c r="E31" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="C32" s="4">
+        <v>5.5150000000000006</v>
+      </c>
+      <c r="D32" s="4">
+        <v>127.185</v>
+      </c>
+      <c r="E32" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="4">
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="C33" s="4">
+        <v>10.89</v>
+      </c>
+      <c r="D33" s="8">
+        <v>125.24999999999999</v>
+      </c>
+      <c r="E33" s="4">
+        <v>0.215</v>
+      </c>
+      <c r="N33" s="4"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="C34" s="4">
+        <v>0.04</v>
+      </c>
+      <c r="D34" s="4">
+        <v>3.6500000000000004</v>
+      </c>
+      <c r="E34" s="4">
+        <v>0</v>
+      </c>
+      <c r="N34" s="4"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="C35" s="4">
+        <v>2.91</v>
+      </c>
+      <c r="D35" s="4">
+        <v>10.93</v>
+      </c>
+      <c r="E35" s="4">
+        <v>0.97</v>
+      </c>
+      <c r="N35" s="4"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="C36" s="4">
+        <v>4.32</v>
+      </c>
+      <c r="D36" s="4">
+        <v>42.045000000000002</v>
+      </c>
+      <c r="E36" s="4">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="N36" s="4"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" s="4">
+        <v>0.255</v>
+      </c>
+      <c r="C37" s="4">
+        <v>12.0075</v>
+      </c>
+      <c r="D37" s="8">
+        <v>130.23500000000001</v>
+      </c>
+      <c r="E37" s="4">
+        <v>0</v>
+      </c>
+      <c r="N37" s="4"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" s="4">
+        <v>0</v>
+      </c>
+      <c r="C38" s="4">
+        <v>0</v>
+      </c>
+      <c r="D38" s="4">
+        <v>8.7200000000000006</v>
+      </c>
+      <c r="E38" s="4">
+        <v>0</v>
+      </c>
+      <c r="N38" s="4"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C39" s="4">
+        <v>5.5E-2</v>
+      </c>
+      <c r="D39" s="4">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="E39" s="4">
+        <v>0</v>
+      </c>
+      <c r="N39" s="4"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="C40" s="4">
+        <v>0.51</v>
+      </c>
+      <c r="D40" s="4">
+        <v>4.9749999999999996</v>
+      </c>
+      <c r="E40" s="4">
+        <v>0.22499999999999998</v>
+      </c>
+      <c r="N40" s="4"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="C41" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="D41" s="4">
+        <v>6.01</v>
+      </c>
+      <c r="E41" s="4">
+        <v>0.18</v>
+      </c>
+      <c r="N41" s="4"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="C42" s="4">
+        <v>4.22</v>
+      </c>
+      <c r="D42" s="4">
+        <v>29.774999999999999</v>
+      </c>
+      <c r="E42" s="4">
+        <v>0</v>
+      </c>
+      <c r="N42" s="4"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" s="4">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="C43" s="4">
+        <v>2.98</v>
+      </c>
+      <c r="D43" s="4">
+        <v>4.4849999999999994</v>
+      </c>
+      <c r="E43" s="4">
+        <v>1.3250000000000002</v>
+      </c>
+      <c r="N43" s="4"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="C44" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="D44" s="4">
+        <v>4.92</v>
+      </c>
+      <c r="E44" s="4">
+        <v>0.61</v>
+      </c>
+      <c r="N44" s="4"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B45" s="4">
+        <v>5.5E-2</v>
+      </c>
+      <c r="C45" s="4">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="D45" s="4">
+        <v>5.71</v>
+      </c>
+      <c r="E45" s="4">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B46" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="C46" s="4">
+        <v>1.1749999999999998</v>
+      </c>
+      <c r="D46" s="4">
+        <v>9.07</v>
+      </c>
+      <c r="E46" s="4">
+        <v>0.44500000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47" s="4">
+        <v>0.09</v>
+      </c>
+      <c r="C47" s="4">
+        <v>0</v>
+      </c>
+      <c r="D47" s="4">
+        <v>9.9700000000000006</v>
+      </c>
+      <c r="E47" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B48" s="4">
+        <v>0.04</v>
+      </c>
+      <c r="C48" s="4">
+        <v>0.97</v>
+      </c>
+      <c r="D48" s="4">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A30" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30" s="4">
-        <v>0.121</v>
-      </c>
-      <c r="C30" s="4">
-        <v>5.4009999999999998</v>
-      </c>
-      <c r="D30" s="4">
-        <v>6.8289999999999997</v>
-      </c>
-      <c r="E30" s="4">
-        <v>0.215</v>
-      </c>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A31" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31" s="4">
-        <v>0.11600000000000001</v>
-      </c>
-      <c r="C31" s="4">
-        <v>0.48499999999999999</v>
-      </c>
-      <c r="D31" s="4">
-        <v>0.67500000000000004</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A32" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32" s="4">
-        <v>0.27900000000000003</v>
-      </c>
-      <c r="C32" s="4">
-        <v>7.6189999999999998</v>
-      </c>
-      <c r="D32" s="4">
-        <v>26.852</v>
-      </c>
-      <c r="E32" s="4">
-        <v>0.60899999999999999</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A33" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B33" s="4">
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="C33" s="4">
-        <v>16.225000000000001</v>
-      </c>
-      <c r="D33" s="8">
-        <v>137.21200000000002</v>
-      </c>
-      <c r="E33" s="4">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="N33" s="4"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A34" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B34" s="4">
-        <v>0.24399999999999999</v>
-      </c>
-      <c r="C34" s="4">
-        <v>0.754</v>
-      </c>
-      <c r="D34" s="4">
-        <v>3.3490000000000002</v>
-      </c>
-      <c r="E34" s="4">
-        <v>0.115</v>
-      </c>
-      <c r="N34" s="4"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A35" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B35" s="4">
-        <v>0.41499999999999998</v>
-      </c>
-      <c r="C35" s="4">
-        <v>3.0539999999999998</v>
-      </c>
-      <c r="D35" s="4">
-        <v>10.302</v>
-      </c>
-      <c r="E35" s="4">
-        <v>1.075</v>
-      </c>
-      <c r="N35" s="4"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A36" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B36" s="4">
-        <v>0.12</v>
-      </c>
-      <c r="C36" s="4">
-        <v>5.3259999999999996</v>
-      </c>
-      <c r="D36" s="4">
-        <v>3.512</v>
-      </c>
-      <c r="E36" s="4">
-        <v>0.19</v>
-      </c>
-      <c r="N36" s="4"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A37" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B37" s="4">
-        <v>0.63600000000000001</v>
-      </c>
-      <c r="C37" s="4">
-        <v>15.170999999999999</v>
-      </c>
-      <c r="D37" s="8">
-        <v>116.464</v>
-      </c>
-      <c r="E37" s="4">
-        <v>8.1000000000000003E-2</v>
-      </c>
-      <c r="N37" s="4"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A38" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B38" s="4">
-        <v>0.217</v>
-      </c>
-      <c r="C38" s="4">
-        <v>0.47699999999999998</v>
-      </c>
-      <c r="D38" s="4">
-        <v>7.7</v>
-      </c>
-      <c r="E38" s="4">
-        <v>0.20499999999999999</v>
-      </c>
-      <c r="N38" s="4"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A39" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B39" s="4">
-        <v>0.128</v>
-      </c>
-      <c r="C39" s="4">
-        <v>0.13500000000000001</v>
-      </c>
-      <c r="D39" s="4">
-        <v>0.82199999999999995</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="N39" s="4"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A40" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B40" s="4">
-        <v>0.26400000000000001</v>
-      </c>
-      <c r="C40" s="4">
-        <v>0.79300000000000004</v>
-      </c>
-      <c r="D40" s="4">
-        <v>5.1630000000000003</v>
-      </c>
-      <c r="E40" s="4">
-        <v>0.312</v>
-      </c>
-      <c r="N40" s="4"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A41" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B41" s="4">
-        <v>0.251</v>
-      </c>
-      <c r="C41" s="4">
-        <v>1.1759999999999999</v>
-      </c>
-      <c r="D41" s="4">
-        <v>4.694</v>
-      </c>
-      <c r="E41" s="4">
-        <v>0.61699999999999999</v>
-      </c>
-      <c r="N41" s="4"/>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A42" s="2" t="s">
+      <c r="E48" s="4">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B42" s="4">
-        <v>0.13500000000000001</v>
-      </c>
-      <c r="C42" s="4">
-        <v>4.601</v>
-      </c>
-      <c r="D42" s="4">
-        <v>3.5539999999999998</v>
-      </c>
-      <c r="E42" s="4">
-        <v>0.16900000000000001</v>
-      </c>
-      <c r="N42" s="4"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A43" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B43" s="4">
-        <v>0.26900000000000002</v>
-      </c>
-      <c r="C43" s="4">
-        <v>3.1030000000000002</v>
-      </c>
-      <c r="D43" s="4">
-        <v>3.944</v>
-      </c>
-      <c r="E43" s="4">
-        <v>1.361</v>
-      </c>
-      <c r="N43" s="4"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A44" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B44" s="4">
-        <v>0.20100000000000001</v>
-      </c>
-      <c r="C44" s="4">
-        <v>1.7250000000000001</v>
-      </c>
-      <c r="D44" s="4">
-        <v>4.5140000000000002</v>
-      </c>
-      <c r="E44" s="4">
-        <v>0.59799999999999998</v>
-      </c>
-      <c r="N44" s="4"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A45" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B45" s="4">
-        <v>0.27800000000000002</v>
-      </c>
-      <c r="C45" s="4">
-        <v>0.78800000000000003</v>
-      </c>
-      <c r="D45" s="4">
-        <v>5.0860000000000003</v>
-      </c>
-      <c r="E45" s="4">
-        <v>0.33700000000000002</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A46" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B46" s="4">
-        <v>0.30199999999999999</v>
-      </c>
-      <c r="C46" s="4">
-        <v>1.8420000000000001</v>
-      </c>
-      <c r="D46" s="4">
-        <v>8.8460000000000001</v>
-      </c>
-      <c r="E46" s="4">
-        <v>0.58299999999999996</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A47" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B47" s="4">
-        <v>0.255</v>
-      </c>
-      <c r="C47" s="4">
-        <v>0.313</v>
-      </c>
-      <c r="D47" s="4">
-        <v>8.3010000000000002</v>
-      </c>
-      <c r="E47" s="4">
-        <v>0.10199999999999999</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A48" s="2" t="s">
+      <c r="B49" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="C49" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="D49" s="4">
+        <v>2.5950000000000002</v>
+      </c>
+      <c r="E49" s="4">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B48" s="4">
-        <v>0.33900000000000002</v>
-      </c>
-      <c r="C48" s="4">
-        <v>1.135</v>
-      </c>
-      <c r="D48" s="4">
-        <v>8.9030000000000005</v>
-      </c>
-      <c r="E48" s="4">
-        <v>0.10100000000000001</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A49" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B49" s="4">
-        <v>0.28100000000000003</v>
-      </c>
-      <c r="C49" s="4">
-        <v>1</v>
-      </c>
-      <c r="D49" s="4">
-        <v>2.3980000000000001</v>
-      </c>
-      <c r="E49" s="4">
-        <v>0.17899999999999999</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A50" s="2" t="s">
+      <c r="B50" s="4">
+        <v>0</v>
+      </c>
+      <c r="C50" s="4">
+        <v>3.34</v>
+      </c>
+      <c r="D50" s="8">
+        <v>93.385000000000005</v>
+      </c>
+      <c r="E50" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="B50" s="4">
-        <v>0.25900000000000001</v>
-      </c>
-      <c r="C50" s="4">
-        <v>4.407</v>
-      </c>
-      <c r="D50" s="8">
-        <v>95.715999999999994</v>
-      </c>
-      <c r="E50" s="4">
-        <v>0.16900000000000001</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A51" s="2"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A52" s="9" t="s">
-        <v>59</v>
       </c>
       <c r="B52" s="9"/>
       <c r="C52" s="9"/>
@@ -2273,508 +2270,372 @@
       <c r="E52" s="9"/>
       <c r="F52" s="9"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="G53" s="1" t="s">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B53" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H53" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I53" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J53" s="1" t="s">
+      <c r="E53" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="G54" s="1" t="s">
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B54" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H54" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I54" s="1" t="s">
+      <c r="D54" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J54" s="1" t="s">
+      <c r="E54" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B55" s="4">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="C55" s="4">
+        <v>5.9</v>
+      </c>
+      <c r="D55" s="4">
+        <v>38.585000000000001</v>
+      </c>
+      <c r="E55" s="4">
+        <v>1.5249999999999999</v>
+      </c>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="4"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B55" s="4">
-        <v>0.16900000000000001</v>
-      </c>
-      <c r="C55" s="4">
-        <v>0.72599999999999998</v>
-      </c>
-      <c r="D55" s="4">
-        <v>3.8130000000000002</v>
-      </c>
-      <c r="E55" s="4">
-        <v>0.20200000000000001</v>
-      </c>
-      <c r="G55" s="4">
-        <f>B55*10</f>
-        <v>1.6900000000000002</v>
-      </c>
-      <c r="H55" s="4">
-        <f t="shared" ref="H55:J66" si="10">C55*10</f>
-        <v>7.26</v>
-      </c>
-      <c r="I55" s="4">
-        <f t="shared" si="10"/>
-        <v>38.130000000000003</v>
-      </c>
-      <c r="J55" s="4">
-        <f t="shared" si="10"/>
-        <v>2.02</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A56" s="2" t="s">
+      <c r="B56" s="4">
+        <v>0.26</v>
+      </c>
+      <c r="C56" s="4">
+        <v>8.14</v>
+      </c>
+      <c r="D56" s="4">
+        <v>19.365000000000002</v>
+      </c>
+      <c r="E56" s="4">
+        <v>0</v>
+      </c>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B56" s="4">
-        <v>0.17599999999999999</v>
-      </c>
-      <c r="C56" s="4">
-        <v>1.0189999999999999</v>
-      </c>
-      <c r="D56" s="4">
-        <v>2.161</v>
-      </c>
-      <c r="E56" s="4">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="G56" s="4">
-        <f t="shared" ref="G56:G66" si="11">B56*10</f>
-        <v>1.7599999999999998</v>
-      </c>
-      <c r="H56" s="4">
-        <f t="shared" si="10"/>
-        <v>10.19</v>
-      </c>
-      <c r="I56" s="4">
-        <f t="shared" si="10"/>
-        <v>21.61</v>
-      </c>
-      <c r="J56" s="4">
-        <f t="shared" si="10"/>
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A57" s="2" t="s">
+      <c r="B57" s="4">
+        <v>0.47</v>
+      </c>
+      <c r="C57" s="4">
+        <v>11.16</v>
+      </c>
+      <c r="D57" s="4">
+        <v>140.35</v>
+      </c>
+      <c r="E57" s="4">
+        <v>0</v>
+      </c>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B57" s="4">
-        <v>0.186</v>
-      </c>
-      <c r="C57" s="4">
-        <v>1.4830000000000001</v>
-      </c>
-      <c r="D57" s="4">
-        <v>14.282999999999999</v>
-      </c>
-      <c r="E57" s="4">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="G57" s="4">
-        <f t="shared" si="11"/>
-        <v>1.8599999999999999</v>
-      </c>
-      <c r="H57" s="4">
-        <f t="shared" si="10"/>
-        <v>14.830000000000002</v>
-      </c>
-      <c r="I57" s="4">
-        <f t="shared" si="10"/>
-        <v>142.82999999999998</v>
-      </c>
-      <c r="J57" s="4">
-        <f t="shared" si="10"/>
-        <v>0.38</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A58" s="2" t="s">
+      <c r="B58" s="4">
+        <v>1.1800000000000002</v>
+      </c>
+      <c r="C58" s="4">
+        <v>12.184999999999999</v>
+      </c>
+      <c r="D58" s="4">
+        <v>100.11500000000001</v>
+      </c>
+      <c r="E58" s="4">
+        <v>1.115</v>
+      </c>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="4"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B59" s="4">
+        <v>1.4849999999999999</v>
+      </c>
+      <c r="C59" s="4">
+        <v>5.4749999999999996</v>
+      </c>
+      <c r="D59" s="4">
+        <v>48.769999999999996</v>
+      </c>
+      <c r="E59" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="4"/>
+      <c r="J59" s="4"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B58" s="4">
-        <v>0.24099999999999999</v>
-      </c>
-      <c r="C58" s="4">
-        <v>1.3879999999999999</v>
-      </c>
-      <c r="D58" s="4">
-        <v>10.545</v>
-      </c>
-      <c r="E58" s="4">
-        <v>0.17599999999999999</v>
-      </c>
-      <c r="G58" s="4">
-        <f t="shared" si="11"/>
-        <v>2.41</v>
-      </c>
-      <c r="H58" s="4">
-        <f t="shared" si="10"/>
-        <v>13.879999999999999</v>
-      </c>
-      <c r="I58" s="4">
-        <f t="shared" si="10"/>
-        <v>105.45</v>
-      </c>
-      <c r="J58" s="4">
-        <f t="shared" si="10"/>
-        <v>1.7599999999999998</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A59" s="2" t="s">
+      <c r="B60" s="4">
+        <v>0.28500000000000003</v>
+      </c>
+      <c r="C60" s="4">
+        <v>6.04</v>
+      </c>
+      <c r="D60" s="4">
+        <v>25.185000000000002</v>
+      </c>
+      <c r="E60" s="4">
+        <v>0.73</v>
+      </c>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="4"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B59" s="4">
-        <v>0.25700000000000001</v>
-      </c>
-      <c r="C59" s="4">
-        <v>0.629</v>
-      </c>
-      <c r="D59" s="4">
-        <v>4.915</v>
-      </c>
-      <c r="E59" s="4">
-        <v>5.8999999999999997E-2</v>
-      </c>
-      <c r="G59" s="4">
-        <f t="shared" si="11"/>
-        <v>2.5700000000000003</v>
-      </c>
-      <c r="H59" s="4">
-        <f t="shared" si="10"/>
-        <v>6.29</v>
-      </c>
-      <c r="I59" s="4">
-        <f t="shared" si="10"/>
-        <v>49.15</v>
-      </c>
-      <c r="J59" s="4">
-        <f t="shared" si="10"/>
-        <v>0.59</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A60" s="2" t="s">
+      <c r="B61" s="4">
+        <v>0.14500000000000002</v>
+      </c>
+      <c r="C61" s="4">
+        <v>10.594999999999999</v>
+      </c>
+      <c r="D61" s="4">
+        <v>27.32</v>
+      </c>
+      <c r="E61" s="4">
+        <v>1.2549999999999999</v>
+      </c>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
+      <c r="J61" s="4"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B60" s="4">
-        <v>0.16300000000000001</v>
-      </c>
-      <c r="C60" s="4">
-        <v>0.69499999999999995</v>
-      </c>
-      <c r="D60" s="4">
-        <v>2.6</v>
-      </c>
-      <c r="E60" s="4">
-        <v>0.112</v>
-      </c>
-      <c r="G60" s="4">
-        <f t="shared" si="11"/>
-        <v>1.6300000000000001</v>
-      </c>
-      <c r="H60" s="4">
-        <f t="shared" si="10"/>
-        <v>6.9499999999999993</v>
-      </c>
-      <c r="I60" s="4">
-        <f t="shared" si="10"/>
-        <v>26</v>
-      </c>
-      <c r="J60" s="4">
-        <f t="shared" si="10"/>
-        <v>1.1200000000000001</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A61" s="2" t="s">
+      <c r="B62" s="4">
+        <v>1.01</v>
+      </c>
+      <c r="C62" s="4">
+        <v>3.83</v>
+      </c>
+      <c r="D62" s="4">
+        <v>43.965000000000003</v>
+      </c>
+      <c r="E62" s="4">
+        <v>0.69</v>
+      </c>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
+      <c r="J62" s="4"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B61" s="4">
-        <v>0.14599999999999999</v>
-      </c>
-      <c r="C61" s="4">
-        <v>1.1850000000000001</v>
-      </c>
-      <c r="D61" s="4">
-        <v>2.8479999999999999</v>
-      </c>
-      <c r="E61" s="4">
-        <v>0.182</v>
-      </c>
-      <c r="G61" s="4">
-        <f t="shared" si="11"/>
-        <v>1.46</v>
-      </c>
-      <c r="H61" s="4">
-        <f t="shared" si="10"/>
-        <v>11.850000000000001</v>
-      </c>
-      <c r="I61" s="4">
-        <f t="shared" si="10"/>
-        <v>28.479999999999997</v>
-      </c>
-      <c r="J61" s="4">
-        <f t="shared" si="10"/>
-        <v>1.8199999999999998</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A62" s="2" t="s">
+      <c r="B63" s="4">
+        <v>1.0449999999999999</v>
+      </c>
+      <c r="C63" s="4">
+        <v>5.9849999999999994</v>
+      </c>
+      <c r="D63" s="4">
+        <v>40.774999999999999</v>
+      </c>
+      <c r="E63" s="4">
+        <v>0.41000000000000003</v>
+      </c>
+      <c r="G63" s="4"/>
+      <c r="H63" s="4"/>
+      <c r="I63" s="4"/>
+      <c r="J63" s="4"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B62" s="4">
-        <v>0.23899999999999999</v>
-      </c>
-      <c r="C62" s="4">
-        <v>0.39700000000000002</v>
-      </c>
-      <c r="D62" s="4">
-        <v>4.5069999999999997</v>
-      </c>
-      <c r="E62" s="4">
-        <v>0.115</v>
-      </c>
-      <c r="G62" s="4">
-        <f t="shared" si="11"/>
-        <v>2.3899999999999997</v>
-      </c>
-      <c r="H62" s="4">
-        <f t="shared" si="10"/>
-        <v>3.97</v>
-      </c>
-      <c r="I62" s="4">
-        <f t="shared" si="10"/>
-        <v>45.069999999999993</v>
-      </c>
-      <c r="J62" s="4">
-        <f t="shared" si="10"/>
-        <v>1.1500000000000001</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A63" s="2" t="s">
+      <c r="B64" s="4">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="C64" s="4">
+        <v>6.2050000000000001</v>
+      </c>
+      <c r="D64" s="4">
+        <v>26.87</v>
+      </c>
+      <c r="E64" s="4">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+      <c r="I64" s="4"/>
+      <c r="J64" s="4"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B63" s="4">
-        <v>0.24399999999999999</v>
-      </c>
-      <c r="C63" s="4">
-        <v>0.77600000000000002</v>
-      </c>
-      <c r="D63" s="4">
-        <v>4.3479999999999999</v>
-      </c>
-      <c r="E63" s="4">
-        <v>9.2999999999999999E-2</v>
-      </c>
-      <c r="G63" s="4">
-        <f t="shared" si="11"/>
-        <v>2.44</v>
-      </c>
-      <c r="H63" s="4">
-        <f t="shared" si="10"/>
-        <v>7.76</v>
-      </c>
-      <c r="I63" s="4">
-        <f t="shared" si="10"/>
-        <v>43.48</v>
-      </c>
-      <c r="J63" s="4">
-        <f t="shared" si="10"/>
+      <c r="B65" s="4">
+        <v>1</v>
+      </c>
+      <c r="C65" s="4">
+        <v>36.32</v>
+      </c>
+      <c r="D65" s="4">
+        <v>22.64</v>
+      </c>
+      <c r="E65" s="4">
+        <v>0.245</v>
+      </c>
+      <c r="G65" s="4"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="4"/>
+      <c r="J65" s="4"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B66" s="4">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="C66" s="4">
+        <v>20.495000000000001</v>
+      </c>
+      <c r="D66" s="4">
+        <v>105.005</v>
+      </c>
+      <c r="E66" s="4">
         <v>0.92999999999999994</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A64" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B64" s="4">
-        <v>0.222</v>
-      </c>
-      <c r="C64" s="4">
-        <v>0.79600000000000004</v>
-      </c>
-      <c r="D64" s="4">
-        <v>2.8540000000000001</v>
-      </c>
-      <c r="E64" s="4">
-        <v>0.125</v>
-      </c>
-      <c r="G64" s="4">
-        <f t="shared" si="11"/>
-        <v>2.2200000000000002</v>
-      </c>
-      <c r="H64" s="4">
-        <f t="shared" si="10"/>
-        <v>7.9600000000000009</v>
-      </c>
-      <c r="I64" s="4">
-        <f t="shared" si="10"/>
-        <v>28.54</v>
-      </c>
-      <c r="J64" s="4">
-        <f t="shared" si="10"/>
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A65" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B65" s="4">
-        <v>0.19</v>
-      </c>
-      <c r="C65" s="4">
-        <v>2.899</v>
-      </c>
-      <c r="D65" s="4">
-        <v>2.2509999999999999</v>
-      </c>
-      <c r="E65" s="4">
-        <v>7.5999999999999998E-2</v>
-      </c>
-      <c r="G65" s="4">
-        <f t="shared" si="11"/>
-        <v>1.9</v>
-      </c>
-      <c r="H65" s="4">
-        <f t="shared" si="10"/>
-        <v>28.990000000000002</v>
-      </c>
-      <c r="I65" s="4">
-        <f t="shared" si="10"/>
-        <v>22.509999999999998</v>
-      </c>
-      <c r="J65" s="4">
-        <f t="shared" si="10"/>
-        <v>0.76</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A66" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B66" s="4">
-        <v>0.189</v>
-      </c>
-      <c r="C66" s="4">
-        <v>1.409</v>
-      </c>
-      <c r="D66" s="4">
-        <v>9.9920000000000009</v>
-      </c>
-      <c r="E66" s="4">
-        <v>4.2999999999999997E-2</v>
-      </c>
-      <c r="G66" s="4">
-        <f t="shared" si="11"/>
-        <v>1.8900000000000001</v>
-      </c>
-      <c r="H66" s="4">
-        <f t="shared" si="10"/>
-        <v>14.09</v>
-      </c>
-      <c r="I66" s="4">
-        <f t="shared" si="10"/>
-        <v>99.920000000000016</v>
-      </c>
-      <c r="J66" s="4">
-        <f t="shared" si="10"/>
-        <v>0.42999999999999994</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="G66" s="4"/>
+      <c r="H66" s="4"/>
+      <c r="I66" s="4"/>
+      <c r="J66" s="4"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
       <c r="I70" s="4"/>
       <c r="J70" s="4"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
       <c r="I71" s="4"/>
       <c r="J71" s="4"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
       <c r="J72" s="4"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="G73" s="4"/>
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
       <c r="J73" s="4"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="G74" s="4"/>
       <c r="H74" s="4"/>
       <c r="I74" s="4"/>
       <c r="J74" s="4"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="G75" s="4"/>
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
       <c r="J75" s="4"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="G76" s="4"/>
       <c r="H76" s="4"/>
       <c r="I76" s="4"/>
       <c r="J76" s="4"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="G77" s="4"/>
       <c r="H77" s="4"/>
       <c r="I77" s="4"/>
       <c r="J77" s="4"/>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="G78" s="4"/>
       <c r="H78" s="4"/>
       <c r="I78" s="4"/>
       <c r="J78" s="4"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="G79" s="4"/>
       <c r="H79" s="4"/>
       <c r="I79" s="4"/>
       <c r="J79" s="4"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="G80" s="4"/>
       <c r="H80" s="4"/>
       <c r="I80" s="4"/>
       <c r="J80" s="4"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="G81" s="4"/>
       <c r="H81" s="4"/>
@@ -2803,34 +2664,34 @@
       <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -2838,7 +2699,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -2846,7 +2707,7 @@
       <c r="E12" s="7"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -2854,7 +2715,7 @@
       <c r="E13" s="7"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -2862,7 +2723,7 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -2870,7 +2731,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -2878,7 +2739,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -2886,7 +2747,7 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>

</xml_diff>